<commit_message>
Latest state before revisiting
</commit_message>
<xml_diff>
--- a/backend/data/analytics/3_straight.xlsx
+++ b/backend/data/analytics/3_straight.xlsx
@@ -561,7 +561,7 @@
         <v>38</v>
       </c>
       <c r="B5" t="n">
-        <v>64</v>
+        <v>60</v>
       </c>
       <c r="C5" t="n">
         <v>62</v>
@@ -596,10 +596,10 @@
         <v>59</v>
       </c>
       <c r="D6" t="n">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="E6" t="n">
-        <v>73</v>
+        <v>71</v>
       </c>
       <c r="F6" t="n">
         <v>71</v>
@@ -619,16 +619,16 @@
         <v>42</v>
       </c>
       <c r="B7" t="n">
-        <v>56.99999999999999</v>
+        <v>56.00000000000001</v>
       </c>
       <c r="C7" t="n">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="D7" t="n">
-        <v>69</v>
+        <v>70</v>
       </c>
       <c r="E7" t="n">
-        <v>75</v>
+        <v>77</v>
       </c>
       <c r="F7" t="n">
         <v>62</v>
@@ -648,10 +648,10 @@
         <v>44</v>
       </c>
       <c r="B8" t="n">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="C8" t="n">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="D8" t="n">
         <v>66</v>
@@ -660,7 +660,7 @@
         <v>65</v>
       </c>
       <c r="F8" t="n">
-        <v>74</v>
+        <v>71</v>
       </c>
       <c r="G8" t="n">
         <v>75</v>
@@ -677,7 +677,7 @@
         <v>46</v>
       </c>
       <c r="B9" t="n">
-        <v>44</v>
+        <v>46</v>
       </c>
       <c r="C9" t="n">
         <v>62</v>
@@ -686,10 +686,10 @@
         <v>66</v>
       </c>
       <c r="E9" t="n">
-        <v>78</v>
+        <v>76</v>
       </c>
       <c r="F9" t="n">
-        <v>72</v>
+        <v>74</v>
       </c>
       <c r="G9" t="n">
         <v>33</v>
@@ -712,7 +712,7 @@
         <v>65</v>
       </c>
       <c r="D10" t="n">
-        <v>67</v>
+        <v>68</v>
       </c>
       <c r="E10" t="n">
         <v>64</v>
@@ -770,7 +770,7 @@
         <v>63</v>
       </c>
       <c r="D12" t="n">
-        <v>67</v>
+        <v>68</v>
       </c>
       <c r="E12" t="n">
         <v>50</v>
@@ -796,7 +796,7 @@
         <v>43</v>
       </c>
       <c r="C13" t="n">
-        <v>73</v>
+        <v>71</v>
       </c>
       <c r="D13" t="n">
         <v>70</v>
@@ -1104,7 +1104,7 @@
         <v>38</v>
       </c>
       <c r="B5" t="n">
-        <v>14</v>
+        <v>15</v>
       </c>
       <c r="C5" t="n">
         <v>50</v>
@@ -1139,10 +1139,10 @@
         <v>179</v>
       </c>
       <c r="D6" t="n">
-        <v>93</v>
+        <v>94</v>
       </c>
       <c r="E6" t="n">
-        <v>26</v>
+        <v>28</v>
       </c>
       <c r="F6" t="n">
         <v>14</v>
@@ -1162,16 +1162,16 @@
         <v>42</v>
       </c>
       <c r="B7" t="n">
-        <v>35</v>
+        <v>36</v>
       </c>
       <c r="C7" t="n">
-        <v>145</v>
+        <v>148</v>
       </c>
       <c r="D7" t="n">
-        <v>85</v>
+        <v>88</v>
       </c>
       <c r="E7" t="n">
-        <v>24</v>
+        <v>26</v>
       </c>
       <c r="F7" t="n">
         <v>13</v>
@@ -1191,19 +1191,19 @@
         <v>44</v>
       </c>
       <c r="B8" t="n">
-        <v>78</v>
+        <v>79</v>
       </c>
       <c r="C8" t="n">
-        <v>328</v>
+        <v>332</v>
       </c>
       <c r="D8" t="n">
-        <v>210</v>
+        <v>214</v>
       </c>
       <c r="E8" t="n">
         <v>92</v>
       </c>
       <c r="F8" t="n">
-        <v>34</v>
+        <v>35</v>
       </c>
       <c r="G8" t="n">
         <v>8</v>
@@ -1220,19 +1220,19 @@
         <v>46</v>
       </c>
       <c r="B9" t="n">
-        <v>34</v>
+        <v>35</v>
       </c>
       <c r="C9" t="n">
-        <v>184</v>
+        <v>188</v>
       </c>
       <c r="D9" t="n">
-        <v>101</v>
+        <v>104</v>
       </c>
       <c r="E9" t="n">
-        <v>36</v>
+        <v>38</v>
       </c>
       <c r="F9" t="n">
-        <v>18</v>
+        <v>19</v>
       </c>
       <c r="G9" t="n">
         <v>3</v>
@@ -1252,10 +1252,10 @@
         <v>71</v>
       </c>
       <c r="C10" t="n">
-        <v>252</v>
+        <v>254</v>
       </c>
       <c r="D10" t="n">
-        <v>169</v>
+        <v>171</v>
       </c>
       <c r="E10" t="n">
         <v>66</v>
@@ -1313,7 +1313,7 @@
         <v>89</v>
       </c>
       <c r="D12" t="n">
-        <v>61</v>
+        <v>63</v>
       </c>
       <c r="E12" t="n">
         <v>22</v>
@@ -1339,7 +1339,7 @@
         <v>7</v>
       </c>
       <c r="C13" t="n">
-        <v>55</v>
+        <v>56</v>
       </c>
       <c r="D13" t="n">
         <v>30</v>
@@ -1583,7 +1583,7 @@
         <v>38</v>
       </c>
       <c r="B3" t="n">
-        <v>67</v>
+        <v>50</v>
       </c>
       <c r="C3" t="n">
         <v>25</v>
@@ -1615,10 +1615,10 @@
         <v>44</v>
       </c>
       <c r="D4" t="n">
-        <v>61</v>
+        <v>59</v>
       </c>
       <c r="E4" t="n">
-        <v>75</v>
+        <v>70</v>
       </c>
       <c r="F4" t="n">
         <v>0</v>
@@ -1635,13 +1635,13 @@
         <v>42</v>
       </c>
       <c r="B5" t="n">
-        <v>57.99999999999999</v>
+        <v>54</v>
       </c>
       <c r="C5" t="n">
-        <v>63</v>
+        <v>61</v>
       </c>
       <c r="D5" t="n">
-        <v>67</v>
+        <v>70</v>
       </c>
       <c r="E5" t="n">
         <v>100</v>
@@ -1661,19 +1661,19 @@
         <v>44</v>
       </c>
       <c r="B6" t="n">
-        <v>60</v>
+        <v>57.99999999999999</v>
       </c>
       <c r="C6" t="n">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="D6" t="n">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="E6" t="n">
         <v>85</v>
       </c>
       <c r="F6" t="n">
-        <v>80</v>
+        <v>75</v>
       </c>
       <c r="G6" t="n">
         <v>75</v>
@@ -1687,19 +1687,19 @@
         <v>46</v>
       </c>
       <c r="B7" t="n">
-        <v>54</v>
+        <v>56.99999999999999</v>
       </c>
       <c r="C7" t="n">
-        <v>59</v>
+        <v>57.99999999999999</v>
       </c>
       <c r="D7" t="n">
-        <v>63</v>
+        <v>64</v>
       </c>
       <c r="E7" t="n">
-        <v>79</v>
+        <v>76</v>
       </c>
       <c r="F7" t="n">
-        <v>56.00000000000001</v>
+        <v>60</v>
       </c>
       <c r="G7" t="n">
         <v>0</v>
@@ -1719,7 +1719,7 @@
         <v>72</v>
       </c>
       <c r="D8" t="n">
-        <v>62</v>
+        <v>63</v>
       </c>
       <c r="E8" t="n">
         <v>70</v>
@@ -1771,7 +1771,7 @@
         <v>67</v>
       </c>
       <c r="D10" t="n">
-        <v>83</v>
+        <v>84</v>
       </c>
       <c r="E10" t="n">
         <v>38</v>
@@ -1794,7 +1794,7 @@
         <v>50</v>
       </c>
       <c r="C11" t="n">
-        <v>63</v>
+        <v>61</v>
       </c>
       <c r="D11" t="n">
         <v>71</v>
@@ -2020,7 +2020,7 @@
         <v>38</v>
       </c>
       <c r="B3" t="n">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="C3" t="n">
         <v>4</v>
@@ -2052,10 +2052,10 @@
         <v>43</v>
       </c>
       <c r="D4" t="n">
-        <v>28</v>
+        <v>29</v>
       </c>
       <c r="E4" t="n">
-        <v>8</v>
+        <v>10</v>
       </c>
       <c r="F4" t="n">
         <v>2</v>
@@ -2072,16 +2072,16 @@
         <v>42</v>
       </c>
       <c r="B5" t="n">
-        <v>12</v>
+        <v>13</v>
       </c>
       <c r="C5" t="n">
-        <v>38</v>
+        <v>41</v>
       </c>
       <c r="D5" t="n">
-        <v>27</v>
+        <v>30</v>
       </c>
       <c r="E5" t="n">
-        <v>7</v>
+        <v>9</v>
       </c>
       <c r="F5" t="n">
         <v>5</v>
@@ -2098,19 +2098,19 @@
         <v>44</v>
       </c>
       <c r="B6" t="n">
-        <v>25</v>
+        <v>26</v>
       </c>
       <c r="C6" t="n">
-        <v>98</v>
+        <v>102</v>
       </c>
       <c r="D6" t="n">
-        <v>74</v>
+        <v>78</v>
       </c>
       <c r="E6" t="n">
         <v>34</v>
       </c>
       <c r="F6" t="n">
-        <v>15</v>
+        <v>16</v>
       </c>
       <c r="G6" t="n">
         <v>4</v>
@@ -2124,19 +2124,19 @@
         <v>46</v>
       </c>
       <c r="B7" t="n">
-        <v>13</v>
+        <v>14</v>
       </c>
       <c r="C7" t="n">
-        <v>56</v>
+        <v>60</v>
       </c>
       <c r="D7" t="n">
-        <v>41</v>
+        <v>44</v>
       </c>
       <c r="E7" t="n">
-        <v>19</v>
+        <v>21</v>
       </c>
       <c r="F7" t="n">
-        <v>9</v>
+        <v>10</v>
       </c>
       <c r="G7" t="n">
         <v>1</v>
@@ -2153,10 +2153,10 @@
         <v>33</v>
       </c>
       <c r="C8" t="n">
-        <v>93</v>
+        <v>95</v>
       </c>
       <c r="D8" t="n">
-        <v>69</v>
+        <v>71</v>
       </c>
       <c r="E8" t="n">
         <v>20</v>
@@ -2208,7 +2208,7 @@
         <v>54</v>
       </c>
       <c r="D10" t="n">
-        <v>29</v>
+        <v>31</v>
       </c>
       <c r="E10" t="n">
         <v>13</v>
@@ -2231,7 +2231,7 @@
         <v>4</v>
       </c>
       <c r="C11" t="n">
-        <v>27</v>
+        <v>28</v>
       </c>
       <c r="D11" t="n">
         <v>14</v>

</xml_diff>